<commit_message>
Added more stuff to purchase tracking sheet
</commit_message>
<xml_diff>
--- a/reports/funding/Cost Breakdown.xlsx
+++ b/reports/funding/Cost Breakdown.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>Group Name:</t>
   </si>
@@ -70,21 +70,6 @@
     <t>Raspberry Pi 3 Model B Starter Kit</t>
   </si>
   <si>
-    <t>Spent- Not from funding</t>
-  </si>
-  <si>
-    <t>Arduino Stuff</t>
-  </si>
-  <si>
-    <t>Total (Taxes Included)</t>
-  </si>
-  <si>
-    <t>Wire Stripper, flashlight, drawers, screwdrivers</t>
-  </si>
-  <si>
-    <t>Miscellaneous electric components</t>
-  </si>
-  <si>
     <t>Z-Wave Controller Stick</t>
   </si>
   <si>
@@ -98,6 +83,12 @@
   </si>
   <si>
     <t>Sonos Play 1</t>
+  </si>
+  <si>
+    <t>Aeotec Zwave Smart Switch</t>
+  </si>
+  <si>
+    <t>Everspring Compact Motion Sensor</t>
   </si>
 </sst>
 </file>
@@ -107,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,8 +137,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +156,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -181,11 +184,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -205,8 +209,10 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -486,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,22 +511,22 @@
     <col min="14" max="14" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="3" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -543,7 +549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -564,44 +570,89 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="D7" s="4">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="E7" s="4">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="F7" s="4">
+        <v>84.73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>36.090000000000003</v>
+      </c>
+      <c r="D8" s="4">
+        <v>36.090000000000003</v>
+      </c>
+      <c r="E8" s="4">
+        <v>9.59</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="D9" s="4">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="E9" s="4">
+        <v>20.39</v>
+      </c>
+      <c r="F9" s="4">
+        <v>90.38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="M10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N10">
-        <v>240.63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C10" s="4">
+        <v>54.99</v>
+      </c>
+      <c r="D10" s="4">
+        <v>109.88</v>
+      </c>
+      <c r="E10" s="4">
+        <v>14.3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>124.28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -618,26 +669,38 @@
       <c r="F11" s="4">
         <v>288.14</v>
       </c>
-      <c r="M11" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11">
-        <v>32.159999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N12">
-        <v>18.48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N13">
-        <f>SUM(N10:N12)</f>
-        <v>291.27</v>
-      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="D12" s="4">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="F12" s="9">
+        <v>141.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>44.99</v>
+      </c>
+      <c r="D13" s="4">
+        <v>44.99</v>
+      </c>
+      <c r="F13" s="9"/>
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28" s="8" t="s">
@@ -645,7 +708,7 @@
       </c>
       <c r="F28" s="4">
         <f>SUM(F6:F27)</f>
-        <v>378.51</v>
+        <v>864.80000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added thermostat to cost breakdown
</commit_message>
<xml_diff>
--- a/reports/funding/Cost Breakdown.xlsx
+++ b/reports/funding/Cost Breakdown.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Group Name:</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Everspring Compact Motion Sensor</t>
+  </si>
+  <si>
+    <t>Radio Thermostat Zwave Plus Auotomation Thermostat</t>
   </si>
 </sst>
 </file>
@@ -98,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,15 +140,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,11 +152,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -184,10 +175,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -209,10 +199,9 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
+  <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -484,7 +473,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -492,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,22 +500,22 @@
     <col min="14" max="14" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -549,7 +538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -570,7 +559,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -590,7 +579,7 @@
         <v>84.73</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -609,8 +598,9 @@
       <c r="F8" s="4">
         <v>45.68</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -629,8 +619,9 @@
       <c r="F9" s="4">
         <v>90.38</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -649,8 +640,9 @@
       <c r="F10" s="4">
         <v>124.28</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -669,8 +661,9 @@
       <c r="F11" s="4">
         <v>288.14</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -683,11 +676,15 @@
       <c r="D12" s="4">
         <v>69.989999999999995</v>
       </c>
-      <c r="F12" s="9">
-        <v>141.22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="4">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F12" s="4">
+        <f>D12+E12</f>
+        <v>79.789999999999992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -700,7 +697,33 @@
       <c r="D13" s="4">
         <v>44.99</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="E13" s="4">
+        <v>16.29</v>
+      </c>
+      <c r="F13" s="9">
+        <f>D13+E13</f>
+        <v>61.28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>99.99</v>
+      </c>
+      <c r="D14" s="4">
+        <v>99.99</v>
+      </c>
+      <c r="E14" s="4">
+        <v>24.29</v>
+      </c>
+      <c r="F14" s="4">
+        <v>124.28</v>
+      </c>
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28" s="8" t="s">
@@ -708,7 +731,7 @@
       </c>
       <c r="F28" s="4">
         <f>SUM(F6:F27)</f>
-        <v>864.80000000000007</v>
+        <v>988.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>